<commit_message>
Updated Read.me with final conclusions on optimized dino bot
</commit_message>
<xml_diff>
--- a/DataAnalysis.xlsx
+++ b/DataAnalysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b4a5232a0414c816/Desktop/CS/Projects/AI/DinoBot-NEAT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="14_{67726723-4F05-45C4-8343-ACB0C14EEF74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{501689F8-0B97-4F80-8D7C-357FA1F47696}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="14_{67726723-4F05-45C4-8343-ACB0C14EEF74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A764B5D-E1C3-49E9-95EC-3CF532B5D419}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2640" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{F16A38F1-B42C-4B58-9450-487B8984C1BF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{F16A38F1-B42C-4B58-9450-487B8984C1BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Population Analysis" sheetId="1" r:id="rId1"/>
@@ -190,7 +190,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -262,30 +262,6 @@
       <sz val="12"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFCCCCCC"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="11">
@@ -377,7 +353,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -422,18 +398,10 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7846,154 +7814,154 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>392</c:v>
+                  <c:v>451.3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>686.33333333333337</c:v>
+                  <c:v>949.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>734.33333333333337</c:v>
+                  <c:v>837.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>629</c:v>
+                  <c:v>1097.5999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>635.66666666666663</c:v>
+                  <c:v>1030.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>837.33333333333337</c:v>
+                  <c:v>1182</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>855.33333333333337</c:v>
+                  <c:v>1224.7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>910.66666666666663</c:v>
+                  <c:v>1263.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>743</c:v>
+                  <c:v>1128.3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>691.33333333333337</c:v>
+                  <c:v>1167.0999999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>644.33333333333337</c:v>
+                  <c:v>1219.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>793.33333333333337</c:v>
+                  <c:v>1201</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>873.66666666666663</c:v>
+                  <c:v>1261.5999999999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>888</c:v>
+                  <c:v>1258.7</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>786</c:v>
+                  <c:v>1225.4000000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>791.66666666666663</c:v>
+                  <c:v>1258.5999999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1169.3333333333333</c:v>
+                  <c:v>1354.7</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>854.33333333333337</c:v>
+                  <c:v>1289.5999999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1005.6666666666666</c:v>
+                  <c:v>1376.2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>970.66666666666663</c:v>
+                  <c:v>1378.7</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>764.33333333333337</c:v>
+                  <c:v>1343.8</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1119</c:v>
+                  <c:v>1464.5</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>671</c:v>
+                  <c:v>1665.9</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>936.66666666666663</c:v>
+                  <c:v>1962.5</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>968</c:v>
+                  <c:v>2086.1999999999998</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>967.33333333333337</c:v>
+                  <c:v>2064.6999999999998</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>931</c:v>
+                  <c:v>1956.5</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1786</c:v>
+                  <c:v>2277.1</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1760.6666666666667</c:v>
+                  <c:v>2224.6999999999998</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1314.3333333333333</c:v>
+                  <c:v>2080.6</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2179.6666666666665</c:v>
+                  <c:v>2392</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1086.6666666666667</c:v>
+                  <c:v>2088</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1152</c:v>
+                  <c:v>2168.8000000000002</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>791.33333333333337</c:v>
+                  <c:v>1938.2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>820.33333333333337</c:v>
+                  <c:v>2028.1</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>921</c:v>
+                  <c:v>2007.9</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>880.66666666666663</c:v>
+                  <c:v>2047.3</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>774.33333333333337</c:v>
+                  <c:v>1996.3</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>887.33333333333337</c:v>
+                  <c:v>2004.1</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>881.66666666666663</c:v>
+                  <c:v>2059.4</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>853</c:v>
+                  <c:v>2041.7</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>932.33333333333337</c:v>
+                  <c:v>2021.7</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>981.33333333333337</c:v>
+                  <c:v>2071.5</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>738.33333333333337</c:v>
+                  <c:v>2022.4</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>955.33333333333337</c:v>
+                  <c:v>2055.1999999999998</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>765.66666666666663</c:v>
+                  <c:v>1982.6</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>583.66666666666663</c:v>
+                  <c:v>1938.4</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>691.66666666666663</c:v>
+                  <c:v>2015.6</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>910</c:v>
+                  <c:v>1978</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>957.66666666666663</c:v>
+                  <c:v>2037.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12911,6 +12879,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -13230,7 +13202,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{900E8F99-93E9-4FEE-AE22-1E57C01964FE}">
   <dimension ref="A1:AV104"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" zoomScale="59" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="K12" zoomScale="59" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AF59" sqref="AF59"/>
     </sheetView>
   </sheetViews>
@@ -21360,8 +21332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CA6133C-7B8D-4CE6-BC4F-0E80738E6184}">
   <dimension ref="A1:BC315"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K17" zoomScale="64" zoomScaleNormal="72" workbookViewId="0">
-      <selection activeCell="AG63" sqref="AG63"/>
+    <sheetView tabSelected="1" topLeftCell="P38" zoomScale="64" zoomScaleNormal="72" workbookViewId="0">
+      <selection activeCell="AQ65" sqref="AQ65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21382,7 +21354,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:55" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:55" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>32</v>
       </c>
@@ -21442,12 +21414,12 @@
       <c r="AU4" s="4"/>
       <c r="AV4" s="4"/>
       <c r="AW4" s="5"/>
-      <c r="AX4" s="22"/>
-      <c r="AY4" s="22"/>
-      <c r="AZ4" s="22"/>
-      <c r="BA4" s="22"/>
-      <c r="BB4" s="22"/>
-      <c r="BC4" s="22"/>
+      <c r="AX4" s="5"/>
+      <c r="AY4" s="5"/>
+      <c r="AZ4" s="5"/>
+      <c r="BA4" s="5"/>
+      <c r="BB4" s="5"/>
+      <c r="BC4" s="5"/>
     </row>
     <row r="5" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
@@ -21616,7 +21588,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="16">
         <v>152</v>
       </c>
@@ -21712,7 +21684,7 @@
       <c r="AE6" s="21">
         <v>233</v>
       </c>
-      <c r="AF6" s="23">
+      <c r="AF6" s="21">
         <v>234</v>
       </c>
       <c r="AG6" s="19">
@@ -21753,28 +21725,42 @@
         <f t="shared" ref="AR6:AR37" si="0">AVERAGE(AH6:AQ6)</f>
         <v>365.2</v>
       </c>
-      <c r="AS6" s="24">
+      <c r="AS6" s="22">
         <v>233</v>
       </c>
-      <c r="AT6" s="24">
+      <c r="AT6" s="22">
         <v>439</v>
       </c>
-      <c r="AU6" s="25">
+      <c r="AU6" s="22">
         <v>504</v>
       </c>
-      <c r="AV6" s="26"/>
-      <c r="AW6" s="26"/>
-      <c r="AX6" s="26"/>
-      <c r="AY6" s="26"/>
-      <c r="AZ6" s="26"/>
-      <c r="BA6" s="26"/>
-      <c r="BB6" s="26"/>
-      <c r="BC6" s="27">
+      <c r="AV6" s="22">
+        <v>1065</v>
+      </c>
+      <c r="AW6" s="22">
+        <v>693</v>
+      </c>
+      <c r="AX6" s="22">
+        <v>232</v>
+      </c>
+      <c r="AY6" s="22">
+        <v>374</v>
+      </c>
+      <c r="AZ6" s="22">
+        <v>303</v>
+      </c>
+      <c r="BA6" s="22">
+        <v>438</v>
+      </c>
+      <c r="BB6" s="22">
+        <v>232</v>
+      </c>
+      <c r="BC6" s="19">
         <f>AVERAGE(AS6:BB6)</f>
-        <v>392</v>
+        <v>451.3</v>
       </c>
     </row>
-    <row r="7" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="16">
         <v>152</v>
       </c>
@@ -21870,7 +21856,7 @@
       <c r="AE7" s="21">
         <v>231</v>
       </c>
-      <c r="AF7" s="23">
+      <c r="AF7" s="21">
         <v>232</v>
       </c>
       <c r="AG7" s="19">
@@ -21911,28 +21897,42 @@
         <f t="shared" si="0"/>
         <v>392.1</v>
       </c>
-      <c r="AS7" s="24">
+      <c r="AS7" s="22">
         <v>505</v>
       </c>
-      <c r="AT7" s="24">
+      <c r="AT7" s="22">
         <v>807</v>
       </c>
-      <c r="AU7" s="25">
+      <c r="AU7" s="22">
         <v>747</v>
       </c>
-      <c r="AV7" s="26"/>
-      <c r="AW7" s="26"/>
-      <c r="AX7" s="26"/>
-      <c r="AY7" s="26"/>
-      <c r="AZ7" s="26"/>
-      <c r="BA7" s="26"/>
-      <c r="BB7" s="26"/>
-      <c r="BC7" s="27">
+      <c r="AV7" s="22">
+        <v>911</v>
+      </c>
+      <c r="AW7" s="22">
+        <v>1825</v>
+      </c>
+      <c r="AX7" s="22">
+        <v>570</v>
+      </c>
+      <c r="AY7" s="22">
+        <v>1555</v>
+      </c>
+      <c r="AZ7" s="22">
+        <v>1248</v>
+      </c>
+      <c r="BA7" s="22">
+        <v>631</v>
+      </c>
+      <c r="BB7" s="22">
+        <v>695</v>
+      </c>
+      <c r="BC7" s="19">
         <f t="shared" ref="BC7:BC55" si="4">AVERAGE(AS7:BB7)</f>
-        <v>686.33333333333337</v>
+        <v>949.4</v>
       </c>
     </row>
-    <row r="8" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="16">
         <v>154</v>
       </c>
@@ -22028,7 +22028,7 @@
       <c r="AE8" s="21">
         <v>233</v>
       </c>
-      <c r="AF8" s="23">
+      <c r="AF8" s="21">
         <v>232</v>
       </c>
       <c r="AG8" s="19">
@@ -22069,28 +22069,42 @@
         <f t="shared" si="0"/>
         <v>497.8</v>
       </c>
-      <c r="AS8" s="24">
+      <c r="AS8" s="22">
         <v>501</v>
       </c>
-      <c r="AT8" s="24">
+      <c r="AT8" s="22">
         <v>1011</v>
       </c>
-      <c r="AU8" s="25">
+      <c r="AU8" s="22">
         <v>691</v>
       </c>
-      <c r="AV8" s="26"/>
-      <c r="AW8" s="26"/>
-      <c r="AX8" s="26"/>
-      <c r="AY8" s="26"/>
-      <c r="AZ8" s="26"/>
-      <c r="BA8" s="26"/>
-      <c r="BB8" s="26"/>
-      <c r="BC8" s="27">
+      <c r="AV8" s="22">
+        <v>907</v>
+      </c>
+      <c r="AW8" s="22">
+        <v>2327</v>
+      </c>
+      <c r="AX8" s="22">
+        <v>437</v>
+      </c>
+      <c r="AY8" s="22">
+        <v>741</v>
+      </c>
+      <c r="AZ8" s="22">
+        <v>625</v>
+      </c>
+      <c r="BA8" s="22">
+        <v>438</v>
+      </c>
+      <c r="BB8" s="22">
+        <v>694</v>
+      </c>
+      <c r="BC8" s="19">
         <f t="shared" si="4"/>
-        <v>734.33333333333337</v>
+        <v>837.2</v>
       </c>
     </row>
-    <row r="9" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="16">
         <v>154</v>
       </c>
@@ -22186,7 +22200,7 @@
       <c r="AE9" s="21">
         <v>1250</v>
       </c>
-      <c r="AF9" s="23">
+      <c r="AF9" s="21">
         <v>232</v>
       </c>
       <c r="AG9" s="19">
@@ -22227,28 +22241,42 @@
         <f t="shared" si="0"/>
         <v>659.5</v>
       </c>
-      <c r="AS9" s="24">
+      <c r="AS9" s="22">
         <v>232</v>
       </c>
-      <c r="AT9" s="24">
+      <c r="AT9" s="22">
         <v>908</v>
       </c>
-      <c r="AU9" s="25">
+      <c r="AU9" s="22">
         <v>747</v>
       </c>
-      <c r="AV9" s="26"/>
-      <c r="AW9" s="26"/>
-      <c r="AX9" s="26"/>
-      <c r="AY9" s="26"/>
-      <c r="AZ9" s="26"/>
-      <c r="BA9" s="26"/>
-      <c r="BB9" s="26"/>
-      <c r="BC9" s="27">
+      <c r="AV9" s="22">
+        <v>1011</v>
+      </c>
+      <c r="AW9" s="22">
+        <v>232</v>
+      </c>
+      <c r="AX9" s="22">
+        <v>441</v>
+      </c>
+      <c r="AY9" s="22">
+        <v>1248</v>
+      </c>
+      <c r="AZ9" s="22">
+        <v>688</v>
+      </c>
+      <c r="BA9" s="22">
+        <v>4667</v>
+      </c>
+      <c r="BB9" s="22">
+        <v>802</v>
+      </c>
+      <c r="BC9" s="19">
         <f t="shared" si="4"/>
-        <v>629</v>
+        <v>1097.5999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="16">
         <v>154</v>
       </c>
@@ -22344,7 +22372,7 @@
       <c r="AE10" s="21">
         <v>1210</v>
       </c>
-      <c r="AF10" s="23">
+      <c r="AF10" s="21">
         <v>230</v>
       </c>
       <c r="AG10" s="19">
@@ -22385,28 +22413,42 @@
         <f t="shared" si="0"/>
         <v>773.3</v>
       </c>
-      <c r="AS10" s="24">
+      <c r="AS10" s="22">
         <v>301</v>
       </c>
-      <c r="AT10" s="24">
+      <c r="AT10" s="22">
         <v>914</v>
       </c>
-      <c r="AU10" s="25">
+      <c r="AU10" s="22">
         <v>692</v>
       </c>
-      <c r="AV10" s="26"/>
-      <c r="AW10" s="26"/>
-      <c r="AX10" s="26"/>
-      <c r="AY10" s="26"/>
-      <c r="AZ10" s="26"/>
-      <c r="BA10" s="26"/>
-      <c r="BB10" s="26"/>
-      <c r="BC10" s="27">
+      <c r="AV10" s="22">
+        <v>1063</v>
+      </c>
+      <c r="AW10" s="22">
+        <v>439</v>
+      </c>
+      <c r="AX10" s="22">
+        <v>441</v>
+      </c>
+      <c r="AY10" s="22">
+        <v>231</v>
+      </c>
+      <c r="AZ10" s="22">
+        <v>752</v>
+      </c>
+      <c r="BA10" s="22">
+        <v>4724</v>
+      </c>
+      <c r="BB10" s="22">
+        <v>750</v>
+      </c>
+      <c r="BC10" s="19">
         <f t="shared" si="4"/>
-        <v>635.66666666666663</v>
+        <v>1030.7</v>
       </c>
     </row>
-    <row r="11" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="16">
         <v>154</v>
       </c>
@@ -22502,7 +22544,7 @@
       <c r="AE11" s="21">
         <v>1336</v>
       </c>
-      <c r="AF11" s="23">
+      <c r="AF11" s="21">
         <v>234</v>
       </c>
       <c r="AG11" s="19">
@@ -22543,28 +22585,42 @@
         <f t="shared" si="0"/>
         <v>621.1</v>
       </c>
-      <c r="AS11" s="24">
+      <c r="AS11" s="22">
         <v>439</v>
       </c>
-      <c r="AT11" s="24">
+      <c r="AT11" s="22">
         <v>1063</v>
       </c>
-      <c r="AU11" s="25">
+      <c r="AU11" s="22">
         <v>1010</v>
       </c>
-      <c r="AV11" s="26"/>
-      <c r="AW11" s="26"/>
-      <c r="AX11" s="26"/>
-      <c r="AY11" s="26"/>
-      <c r="AZ11" s="26"/>
-      <c r="BA11" s="26"/>
-      <c r="BB11" s="26"/>
-      <c r="BC11" s="27">
+      <c r="AV11" s="22">
+        <v>1250</v>
+      </c>
+      <c r="AW11" s="22">
+        <v>440</v>
+      </c>
+      <c r="AX11" s="22">
+        <v>510</v>
+      </c>
+      <c r="AY11" s="22">
+        <v>222</v>
+      </c>
+      <c r="AZ11" s="22">
+        <v>1245</v>
+      </c>
+      <c r="BA11" s="22">
+        <v>4726</v>
+      </c>
+      <c r="BB11" s="22">
+        <v>915</v>
+      </c>
+      <c r="BC11" s="19">
         <f t="shared" si="4"/>
-        <v>837.33333333333337</v>
+        <v>1182</v>
       </c>
     </row>
-    <row r="12" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="16">
         <v>153</v>
       </c>
@@ -22660,7 +22716,7 @@
       <c r="AE12" s="21">
         <v>628</v>
       </c>
-      <c r="AF12" s="23">
+      <c r="AF12" s="21">
         <v>912</v>
       </c>
       <c r="AG12" s="19">
@@ -22701,28 +22757,42 @@
         <f t="shared" si="0"/>
         <v>768.1</v>
       </c>
-      <c r="AS12" s="24">
+      <c r="AS12" s="22">
         <v>508</v>
       </c>
-      <c r="AT12" s="24">
+      <c r="AT12" s="22">
         <v>1249</v>
       </c>
-      <c r="AU12" s="25">
+      <c r="AU12" s="22">
         <v>809</v>
       </c>
-      <c r="AV12" s="26"/>
-      <c r="AW12" s="26"/>
-      <c r="AX12" s="26"/>
-      <c r="AY12" s="26"/>
-      <c r="AZ12" s="26"/>
-      <c r="BA12" s="26"/>
-      <c r="BB12" s="26"/>
-      <c r="BC12" s="27">
+      <c r="AV12" s="22">
+        <v>1013</v>
+      </c>
+      <c r="AW12" s="22">
+        <v>1108</v>
+      </c>
+      <c r="AX12" s="22">
+        <v>859</v>
+      </c>
+      <c r="AY12" s="22">
+        <v>297</v>
+      </c>
+      <c r="AZ12" s="22">
+        <v>739</v>
+      </c>
+      <c r="BA12" s="22">
+        <v>4704</v>
+      </c>
+      <c r="BB12" s="22">
+        <v>961</v>
+      </c>
+      <c r="BC12" s="19">
         <f t="shared" si="4"/>
-        <v>855.33333333333337</v>
+        <v>1224.7</v>
       </c>
     </row>
-    <row r="13" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="16">
         <v>225</v>
       </c>
@@ -22818,7 +22888,7 @@
       <c r="AE13" s="21">
         <v>568</v>
       </c>
-      <c r="AF13" s="23">
+      <c r="AF13" s="21">
         <v>1014</v>
       </c>
       <c r="AG13" s="19">
@@ -22859,28 +22929,42 @@
         <f t="shared" si="0"/>
         <v>600.4</v>
       </c>
-      <c r="AS13" s="24">
+      <c r="AS13" s="22">
         <v>909</v>
       </c>
-      <c r="AT13" s="24">
+      <c r="AT13" s="22">
         <v>906</v>
       </c>
-      <c r="AU13" s="25">
+      <c r="AU13" s="22">
         <v>917</v>
       </c>
-      <c r="AV13" s="26"/>
-      <c r="AW13" s="26"/>
-      <c r="AX13" s="26"/>
-      <c r="AY13" s="26"/>
-      <c r="AZ13" s="26"/>
-      <c r="BA13" s="26"/>
-      <c r="BB13" s="26"/>
-      <c r="BC13" s="27">
+      <c r="AV13" s="22">
+        <v>914</v>
+      </c>
+      <c r="AW13" s="22">
+        <v>913</v>
+      </c>
+      <c r="AX13" s="22">
+        <v>1162</v>
+      </c>
+      <c r="AY13" s="22">
+        <v>233</v>
+      </c>
+      <c r="AZ13" s="22">
+        <v>1018</v>
+      </c>
+      <c r="BA13" s="22">
+        <v>4748</v>
+      </c>
+      <c r="BB13" s="22">
+        <v>915</v>
+      </c>
+      <c r="BC13" s="19">
         <f t="shared" si="4"/>
-        <v>910.66666666666663</v>
+        <v>1263.5</v>
       </c>
     </row>
-    <row r="14" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="16">
         <v>230</v>
       </c>
@@ -22976,7 +23060,7 @@
       <c r="AE14" s="21">
         <v>570</v>
       </c>
-      <c r="AF14" s="23">
+      <c r="AF14" s="21">
         <v>914</v>
       </c>
       <c r="AG14" s="19">
@@ -23017,28 +23101,42 @@
         <f t="shared" si="0"/>
         <v>613.70000000000005</v>
       </c>
-      <c r="AS14" s="24">
+      <c r="AS14" s="22">
         <v>810</v>
       </c>
-      <c r="AT14" s="24">
+      <c r="AT14" s="22">
         <v>911</v>
       </c>
-      <c r="AU14" s="25">
+      <c r="AU14" s="22">
         <v>508</v>
       </c>
-      <c r="AV14" s="26"/>
-      <c r="AW14" s="26"/>
-      <c r="AX14" s="26"/>
-      <c r="AY14" s="26"/>
-      <c r="AZ14" s="26"/>
-      <c r="BA14" s="26"/>
-      <c r="BB14" s="26"/>
-      <c r="BC14" s="27">
+      <c r="AV14" s="22">
+        <v>914</v>
+      </c>
+      <c r="AW14" s="22">
+        <v>442</v>
+      </c>
+      <c r="AX14" s="22">
+        <v>911</v>
+      </c>
+      <c r="AY14" s="22">
+        <v>232</v>
+      </c>
+      <c r="AZ14" s="22">
+        <v>964</v>
+      </c>
+      <c r="BA14" s="22">
+        <v>4733</v>
+      </c>
+      <c r="BB14" s="22">
+        <v>858</v>
+      </c>
+      <c r="BC14" s="19">
         <f t="shared" si="4"/>
-        <v>743</v>
+        <v>1128.3</v>
       </c>
     </row>
-    <row r="15" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="16">
         <v>155</v>
       </c>
@@ -23134,7 +23232,7 @@
       <c r="AE15" s="21">
         <v>629</v>
       </c>
-      <c r="AF15" s="23">
+      <c r="AF15" s="21">
         <v>913</v>
       </c>
       <c r="AG15" s="19">
@@ -23175,28 +23273,42 @@
         <f t="shared" si="0"/>
         <v>618.5</v>
       </c>
-      <c r="AS15" s="24">
+      <c r="AS15" s="22">
         <v>626</v>
       </c>
-      <c r="AT15" s="24">
+      <c r="AT15" s="22">
         <v>1010</v>
       </c>
-      <c r="AU15" s="25">
+      <c r="AU15" s="22">
         <v>438</v>
       </c>
-      <c r="AV15" s="26"/>
-      <c r="AW15" s="26"/>
-      <c r="AX15" s="26"/>
-      <c r="AY15" s="26"/>
-      <c r="AZ15" s="26"/>
-      <c r="BA15" s="26"/>
-      <c r="BB15" s="26"/>
-      <c r="BC15" s="27">
+      <c r="AV15" s="22">
+        <v>918</v>
+      </c>
+      <c r="AW15" s="22">
+        <v>688</v>
+      </c>
+      <c r="AX15" s="22">
+        <v>906</v>
+      </c>
+      <c r="AY15" s="22">
+        <v>153</v>
+      </c>
+      <c r="AZ15" s="22">
+        <v>1559</v>
+      </c>
+      <c r="BA15" s="22">
+        <v>4749</v>
+      </c>
+      <c r="BB15" s="22">
+        <v>624</v>
+      </c>
+      <c r="BC15" s="19">
         <f t="shared" si="4"/>
-        <v>691.33333333333337</v>
+        <v>1167.0999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="16">
         <v>158</v>
       </c>
@@ -23292,7 +23404,7 @@
       <c r="AE16" s="21">
         <v>1207</v>
       </c>
-      <c r="AF16" s="23">
+      <c r="AF16" s="21">
         <v>623</v>
       </c>
       <c r="AG16" s="19">
@@ -23333,28 +23445,42 @@
         <f t="shared" si="0"/>
         <v>664.2</v>
       </c>
-      <c r="AS16" s="24">
+      <c r="AS16" s="22">
         <v>682</v>
       </c>
-      <c r="AT16" s="24">
+      <c r="AT16" s="22">
         <v>685</v>
       </c>
-      <c r="AU16" s="25">
+      <c r="AU16" s="22">
         <v>566</v>
       </c>
-      <c r="AV16" s="26"/>
-      <c r="AW16" s="26"/>
-      <c r="AX16" s="26"/>
-      <c r="AY16" s="26"/>
-      <c r="AZ16" s="26"/>
-      <c r="BA16" s="26"/>
-      <c r="BB16" s="26"/>
-      <c r="BC16" s="27">
+      <c r="AV16" s="22">
+        <v>1069</v>
+      </c>
+      <c r="AW16" s="22">
+        <v>912</v>
+      </c>
+      <c r="AX16" s="22">
+        <v>909</v>
+      </c>
+      <c r="AY16" s="22">
+        <v>231</v>
+      </c>
+      <c r="AZ16" s="22">
+        <v>1761</v>
+      </c>
+      <c r="BA16" s="22">
+        <v>4752</v>
+      </c>
+      <c r="BB16" s="22">
+        <v>628</v>
+      </c>
+      <c r="BC16" s="19">
         <f t="shared" si="4"/>
-        <v>644.33333333333337</v>
+        <v>1219.5</v>
       </c>
     </row>
-    <row r="17" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="16">
         <v>154</v>
       </c>
@@ -23450,7 +23576,7 @@
       <c r="AE17" s="21">
         <v>1211</v>
       </c>
-      <c r="AF17" s="23">
+      <c r="AF17" s="21">
         <v>907</v>
       </c>
       <c r="AG17" s="19">
@@ -23491,28 +23617,42 @@
         <f t="shared" si="0"/>
         <v>728.1</v>
       </c>
-      <c r="AS17" s="24">
+      <c r="AS17" s="22">
         <v>1019</v>
       </c>
-      <c r="AT17" s="24">
+      <c r="AT17" s="22">
         <v>856</v>
       </c>
-      <c r="AU17" s="25">
+      <c r="AU17" s="22">
         <v>505</v>
       </c>
-      <c r="AV17" s="26"/>
-      <c r="AW17" s="26"/>
-      <c r="AX17" s="26"/>
-      <c r="AY17" s="26"/>
-      <c r="AZ17" s="26"/>
-      <c r="BA17" s="26"/>
-      <c r="BB17" s="26"/>
-      <c r="BC17" s="27">
+      <c r="AV17" s="22">
+        <v>1064</v>
+      </c>
+      <c r="AW17" s="22">
+        <v>439</v>
+      </c>
+      <c r="AX17" s="22">
+        <v>963</v>
+      </c>
+      <c r="AY17" s="22">
+        <v>691</v>
+      </c>
+      <c r="AZ17" s="22">
+        <v>1012</v>
+      </c>
+      <c r="BA17" s="22">
+        <v>4771</v>
+      </c>
+      <c r="BB17" s="22">
+        <v>690</v>
+      </c>
+      <c r="BC17" s="19">
         <f t="shared" si="4"/>
-        <v>793.33333333333337</v>
+        <v>1201</v>
       </c>
     </row>
-    <row r="18" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="16">
         <v>154</v>
       </c>
@@ -23608,7 +23748,7 @@
       <c r="AE18" s="21">
         <v>1106</v>
       </c>
-      <c r="AF18" s="23">
+      <c r="AF18" s="21">
         <v>1065</v>
       </c>
       <c r="AG18" s="19">
@@ -23649,28 +23789,42 @@
         <f t="shared" si="0"/>
         <v>668.4</v>
       </c>
-      <c r="AS18" s="24">
+      <c r="AS18" s="22">
         <v>1304</v>
       </c>
-      <c r="AT18" s="24">
+      <c r="AT18" s="22">
         <v>629</v>
       </c>
-      <c r="AU18" s="25">
+      <c r="AU18" s="22">
         <v>688</v>
       </c>
-      <c r="AV18" s="26"/>
-      <c r="AW18" s="26"/>
-      <c r="AX18" s="26"/>
-      <c r="AY18" s="26"/>
-      <c r="AZ18" s="26"/>
-      <c r="BA18" s="26"/>
-      <c r="BB18" s="26"/>
-      <c r="BC18" s="27">
+      <c r="AV18" s="22">
+        <v>1209</v>
+      </c>
+      <c r="AW18" s="22">
+        <v>751</v>
+      </c>
+      <c r="AX18" s="22">
+        <v>965</v>
+      </c>
+      <c r="AY18" s="22">
+        <v>857</v>
+      </c>
+      <c r="AZ18" s="22">
+        <v>688</v>
+      </c>
+      <c r="BA18" s="22">
+        <v>4723</v>
+      </c>
+      <c r="BB18" s="22">
+        <v>802</v>
+      </c>
+      <c r="BC18" s="19">
         <f t="shared" si="4"/>
-        <v>873.66666666666663</v>
+        <v>1261.5999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="16">
         <v>153</v>
       </c>
@@ -23766,7 +23920,7 @@
       <c r="AE19" s="21">
         <v>963</v>
       </c>
-      <c r="AF19" s="23">
+      <c r="AF19" s="21">
         <v>913</v>
       </c>
       <c r="AG19" s="19">
@@ -23807,28 +23961,42 @@
         <f t="shared" si="0"/>
         <v>725.7</v>
       </c>
-      <c r="AS19" s="24">
+      <c r="AS19" s="22">
         <v>1117</v>
       </c>
-      <c r="AT19" s="24">
+      <c r="AT19" s="22">
         <v>689</v>
       </c>
-      <c r="AU19" s="25">
+      <c r="AU19" s="22">
         <v>858</v>
       </c>
-      <c r="AV19" s="26"/>
-      <c r="AW19" s="26"/>
-      <c r="AX19" s="26"/>
-      <c r="AY19" s="26"/>
-      <c r="AZ19" s="26"/>
-      <c r="BA19" s="26"/>
-      <c r="BB19" s="26"/>
-      <c r="BC19" s="27">
+      <c r="AV19" s="22">
+        <v>1011</v>
+      </c>
+      <c r="AW19" s="22">
+        <v>910</v>
+      </c>
+      <c r="AX19" s="22">
+        <v>959</v>
+      </c>
+      <c r="AY19" s="22">
+        <v>810</v>
+      </c>
+      <c r="AZ19" s="22">
+        <v>687</v>
+      </c>
+      <c r="BA19" s="22">
+        <v>4809</v>
+      </c>
+      <c r="BB19" s="22">
+        <v>737</v>
+      </c>
+      <c r="BC19" s="19">
         <f t="shared" si="4"/>
-        <v>888</v>
+        <v>1258.7</v>
       </c>
     </row>
-    <row r="20" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="16">
         <v>156</v>
       </c>
@@ -23924,7 +24092,7 @@
       <c r="AE20" s="21">
         <v>965</v>
       </c>
-      <c r="AF20" s="23">
+      <c r="AF20" s="21">
         <v>911</v>
       </c>
       <c r="AG20" s="19">
@@ -23965,28 +24133,42 @@
         <f t="shared" si="0"/>
         <v>810.2</v>
       </c>
-      <c r="AS20" s="24">
+      <c r="AS20" s="22">
         <v>1012</v>
       </c>
-      <c r="AT20" s="24">
+      <c r="AT20" s="22">
         <v>909</v>
       </c>
-      <c r="AU20" s="25">
+      <c r="AU20" s="22">
         <v>437</v>
       </c>
-      <c r="AV20" s="26"/>
-      <c r="AW20" s="26"/>
-      <c r="AX20" s="26"/>
-      <c r="AY20" s="26"/>
-      <c r="AZ20" s="26"/>
-      <c r="BA20" s="26"/>
-      <c r="BB20" s="26"/>
-      <c r="BC20" s="27">
+      <c r="AV20" s="22">
+        <v>1059</v>
+      </c>
+      <c r="AW20" s="22">
+        <v>686</v>
+      </c>
+      <c r="AX20" s="22">
+        <v>1066</v>
+      </c>
+      <c r="AY20" s="22">
+        <v>1061</v>
+      </c>
+      <c r="AZ20" s="22">
+        <v>856</v>
+      </c>
+      <c r="BA20" s="22">
+        <v>4731</v>
+      </c>
+      <c r="BB20" s="22">
+        <v>437</v>
+      </c>
+      <c r="BC20" s="19">
         <f t="shared" si="4"/>
-        <v>786</v>
+        <v>1225.4000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="16">
         <v>227</v>
       </c>
@@ -24082,7 +24264,7 @@
       <c r="AE21" s="21">
         <v>1343</v>
       </c>
-      <c r="AF21" s="23">
+      <c r="AF21" s="21">
         <v>1018</v>
       </c>
       <c r="AG21" s="19">
@@ -24123,28 +24305,42 @@
         <f t="shared" si="0"/>
         <v>756.5</v>
       </c>
-      <c r="AS21" s="24">
+      <c r="AS21" s="22">
         <v>959</v>
       </c>
-      <c r="AT21" s="24">
+      <c r="AT21" s="22">
         <v>911</v>
       </c>
-      <c r="AU21" s="25">
+      <c r="AU21" s="22">
         <v>505</v>
       </c>
-      <c r="AV21" s="26"/>
-      <c r="AW21" s="26"/>
-      <c r="AX21" s="26"/>
-      <c r="AY21" s="26"/>
-      <c r="AZ21" s="26"/>
-      <c r="BA21" s="26"/>
-      <c r="BB21" s="26"/>
-      <c r="BC21" s="27">
+      <c r="AV21" s="22">
+        <v>1203</v>
+      </c>
+      <c r="AW21" s="22">
+        <v>851</v>
+      </c>
+      <c r="AX21" s="22">
+        <v>1248</v>
+      </c>
+      <c r="AY21" s="22">
+        <v>909</v>
+      </c>
+      <c r="AZ21" s="22">
+        <v>750</v>
+      </c>
+      <c r="BA21" s="22">
+        <v>4744</v>
+      </c>
+      <c r="BB21" s="22">
+        <v>506</v>
+      </c>
+      <c r="BC21" s="19">
         <f t="shared" si="4"/>
-        <v>791.66666666666663</v>
+        <v>1258.5999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="16">
         <v>154</v>
       </c>
@@ -24240,7 +24436,7 @@
       <c r="AE22" s="21">
         <v>1012</v>
       </c>
-      <c r="AF22" s="23">
+      <c r="AF22" s="21">
         <v>920</v>
       </c>
       <c r="AG22" s="19">
@@ -24281,28 +24477,42 @@
         <f t="shared" si="0"/>
         <v>696.9</v>
       </c>
-      <c r="AS22" s="24">
+      <c r="AS22" s="22">
         <v>1508</v>
       </c>
-      <c r="AT22" s="24">
+      <c r="AT22" s="22">
         <v>1255</v>
       </c>
-      <c r="AU22" s="25">
+      <c r="AU22" s="22">
         <v>745</v>
       </c>
-      <c r="AV22" s="26"/>
-      <c r="AW22" s="26"/>
-      <c r="AX22" s="26"/>
-      <c r="AY22" s="26"/>
-      <c r="AZ22" s="26"/>
-      <c r="BA22" s="26"/>
-      <c r="BB22" s="26"/>
-      <c r="BC22" s="27">
+      <c r="AV22" s="22">
+        <v>1945</v>
+      </c>
+      <c r="AW22" s="22">
+        <v>630</v>
+      </c>
+      <c r="AX22" s="22">
+        <v>1210</v>
+      </c>
+      <c r="AY22" s="22">
+        <v>373</v>
+      </c>
+      <c r="AZ22" s="22">
+        <v>628</v>
+      </c>
+      <c r="BA22" s="22">
+        <v>4749</v>
+      </c>
+      <c r="BB22" s="22">
+        <v>504</v>
+      </c>
+      <c r="BC22" s="19">
         <f t="shared" si="4"/>
-        <v>1169.3333333333333</v>
+        <v>1354.7</v>
       </c>
     </row>
-    <row r="23" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="16">
         <v>156</v>
       </c>
@@ -24398,7 +24608,7 @@
       <c r="AE23" s="21">
         <v>1010</v>
       </c>
-      <c r="AF23" s="23">
+      <c r="AF23" s="21">
         <v>855</v>
       </c>
       <c r="AG23" s="19">
@@ -24439,28 +24649,42 @@
         <f t="shared" si="0"/>
         <v>796.1</v>
       </c>
-      <c r="AS23" s="24">
+      <c r="AS23" s="22">
         <v>1638</v>
       </c>
-      <c r="AT23" s="24">
+      <c r="AT23" s="22">
         <v>232</v>
       </c>
-      <c r="AU23" s="25">
+      <c r="AU23" s="22">
         <v>693</v>
       </c>
-      <c r="AV23" s="26"/>
-      <c r="AW23" s="26"/>
-      <c r="AX23" s="26"/>
-      <c r="AY23" s="26"/>
-      <c r="AZ23" s="26"/>
-      <c r="BA23" s="26"/>
-      <c r="BB23" s="26"/>
-      <c r="BC23" s="27">
+      <c r="AV23" s="22">
+        <v>1944</v>
+      </c>
+      <c r="AW23" s="22">
+        <v>1210</v>
+      </c>
+      <c r="AX23" s="22">
+        <v>907</v>
+      </c>
+      <c r="AY23" s="22">
+        <v>232</v>
+      </c>
+      <c r="AZ23" s="22">
+        <v>629</v>
+      </c>
+      <c r="BA23" s="22">
+        <v>4783</v>
+      </c>
+      <c r="BB23" s="22">
+        <v>628</v>
+      </c>
+      <c r="BC23" s="19">
         <f t="shared" si="4"/>
-        <v>854.33333333333337</v>
+        <v>1289.5999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="16">
         <v>154</v>
       </c>
@@ -24556,7 +24780,7 @@
       <c r="AE24" s="21">
         <v>631</v>
       </c>
-      <c r="AF24" s="23">
+      <c r="AF24" s="21">
         <v>233</v>
       </c>
       <c r="AG24" s="19">
@@ -24597,28 +24821,42 @@
         <f t="shared" si="0"/>
         <v>750.4</v>
       </c>
-      <c r="AS24" s="24">
+      <c r="AS24" s="22">
         <v>1826</v>
       </c>
-      <c r="AT24" s="24">
+      <c r="AT24" s="22">
         <v>225</v>
       </c>
-      <c r="AU24" s="25">
+      <c r="AU24" s="22">
         <v>966</v>
       </c>
-      <c r="AV24" s="26"/>
-      <c r="AW24" s="26"/>
-      <c r="AX24" s="26"/>
-      <c r="AY24" s="26"/>
-      <c r="AZ24" s="26"/>
-      <c r="BA24" s="26"/>
-      <c r="BB24" s="26"/>
-      <c r="BC24" s="27">
+      <c r="AV24" s="22">
+        <v>1939</v>
+      </c>
+      <c r="AW24" s="22">
+        <v>631</v>
+      </c>
+      <c r="AX24" s="22">
+        <v>1206</v>
+      </c>
+      <c r="AY24" s="22">
+        <v>440</v>
+      </c>
+      <c r="AZ24" s="22">
+        <v>688</v>
+      </c>
+      <c r="BA24" s="22">
+        <v>4828</v>
+      </c>
+      <c r="BB24" s="22">
+        <v>1013</v>
+      </c>
+      <c r="BC24" s="19">
         <f t="shared" si="4"/>
-        <v>1005.6666666666666</v>
+        <v>1376.2</v>
       </c>
     </row>
-    <row r="25" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="16">
         <v>156</v>
       </c>
@@ -24714,7 +24952,7 @@
       <c r="AE25" s="21">
         <v>807</v>
       </c>
-      <c r="AF25" s="23">
+      <c r="AF25" s="21">
         <v>232</v>
       </c>
       <c r="AG25" s="19">
@@ -24755,28 +24993,42 @@
         <f t="shared" si="0"/>
         <v>731.8</v>
       </c>
-      <c r="AS25" s="24">
+      <c r="AS25" s="22">
         <v>1826</v>
       </c>
-      <c r="AT25" s="24">
+      <c r="AT25" s="22">
         <v>231</v>
       </c>
-      <c r="AU25" s="25">
+      <c r="AU25" s="22">
         <v>855</v>
       </c>
-      <c r="AV25" s="26"/>
-      <c r="AW25" s="26"/>
-      <c r="AX25" s="26"/>
-      <c r="AY25" s="26"/>
-      <c r="AZ25" s="26"/>
-      <c r="BA25" s="26"/>
-      <c r="BB25" s="26"/>
-      <c r="BC25" s="27">
+      <c r="AV25" s="22">
+        <v>1978</v>
+      </c>
+      <c r="AW25" s="22">
+        <v>849</v>
+      </c>
+      <c r="AX25" s="22">
+        <v>1210</v>
+      </c>
+      <c r="AY25" s="22">
+        <v>694</v>
+      </c>
+      <c r="AZ25" s="22">
+        <v>748</v>
+      </c>
+      <c r="BA25" s="22">
+        <v>4706</v>
+      </c>
+      <c r="BB25" s="22">
+        <v>690</v>
+      </c>
+      <c r="BC25" s="19">
         <f t="shared" si="4"/>
-        <v>970.66666666666663</v>
+        <v>1378.7</v>
       </c>
     </row>
-    <row r="26" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="16">
         <v>154</v>
       </c>
@@ -24872,7 +25124,7 @@
       <c r="AE26" s="21">
         <v>966</v>
       </c>
-      <c r="AF26" s="23">
+      <c r="AF26" s="21">
         <v>233</v>
       </c>
       <c r="AG26" s="19">
@@ -24913,28 +25165,42 @@
         <f t="shared" si="0"/>
         <v>742.7</v>
       </c>
-      <c r="AS26" s="24">
+      <c r="AS26" s="22">
         <v>1253</v>
       </c>
-      <c r="AT26" s="24">
+      <c r="AT26" s="22">
         <v>232</v>
       </c>
-      <c r="AU26" s="25">
+      <c r="AU26" s="22">
         <v>808</v>
       </c>
-      <c r="AV26" s="26"/>
-      <c r="AW26" s="26"/>
-      <c r="AX26" s="26"/>
-      <c r="AY26" s="26"/>
-      <c r="AZ26" s="26"/>
-      <c r="BA26" s="26"/>
-      <c r="BB26" s="26"/>
-      <c r="BC26" s="27">
+      <c r="AV26" s="22">
+        <v>1204</v>
+      </c>
+      <c r="AW26" s="22">
+        <v>1016</v>
+      </c>
+      <c r="AX26" s="22">
+        <v>1066</v>
+      </c>
+      <c r="AY26" s="22">
+        <v>440</v>
+      </c>
+      <c r="AZ26" s="22">
+        <v>1758</v>
+      </c>
+      <c r="BA26" s="22">
+        <v>4698</v>
+      </c>
+      <c r="BB26" s="22">
+        <v>963</v>
+      </c>
+      <c r="BC26" s="19">
         <f t="shared" si="4"/>
-        <v>764.33333333333337</v>
+        <v>1343.8</v>
       </c>
     </row>
-    <row r="27" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="16">
         <v>155</v>
       </c>
@@ -25030,7 +25296,7 @@
       <c r="AE27" s="21">
         <v>627</v>
       </c>
-      <c r="AF27" s="23">
+      <c r="AF27" s="21">
         <v>232</v>
       </c>
       <c r="AG27" s="19">
@@ -25071,28 +25337,42 @@
         <f t="shared" si="0"/>
         <v>839.9</v>
       </c>
-      <c r="AS27" s="24">
+      <c r="AS27" s="22">
         <v>1829</v>
       </c>
-      <c r="AT27" s="24">
+      <c r="AT27" s="22">
         <v>231</v>
       </c>
-      <c r="AU27" s="25">
+      <c r="AU27" s="22">
         <v>1297</v>
       </c>
-      <c r="AV27" s="26"/>
-      <c r="AW27" s="26"/>
-      <c r="AX27" s="26"/>
-      <c r="AY27" s="26"/>
-      <c r="AZ27" s="26"/>
-      <c r="BA27" s="26"/>
-      <c r="BB27" s="26"/>
-      <c r="BC27" s="27">
+      <c r="AV27" s="22">
+        <v>1943</v>
+      </c>
+      <c r="AW27" s="22">
+        <v>966</v>
+      </c>
+      <c r="AX27" s="22">
+        <v>911</v>
+      </c>
+      <c r="AY27" s="22">
+        <v>1119</v>
+      </c>
+      <c r="AZ27" s="22">
+        <v>631</v>
+      </c>
+      <c r="BA27" s="22">
+        <v>4753</v>
+      </c>
+      <c r="BB27" s="22">
+        <v>965</v>
+      </c>
+      <c r="BC27" s="19">
         <f t="shared" si="4"/>
-        <v>1119</v>
+        <v>1464.5</v>
       </c>
     </row>
-    <row r="28" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="16">
         <v>159</v>
       </c>
@@ -25188,7 +25468,7 @@
       <c r="AE28" s="21">
         <v>688</v>
       </c>
-      <c r="AF28" s="23">
+      <c r="AF28" s="21">
         <v>232</v>
       </c>
       <c r="AG28" s="19">
@@ -25229,28 +25509,42 @@
         <f t="shared" si="0"/>
         <v>727.4</v>
       </c>
-      <c r="AS28" s="24">
+      <c r="AS28" s="22">
         <v>1630</v>
       </c>
-      <c r="AT28" s="24">
+      <c r="AT28" s="22">
         <v>151</v>
       </c>
-      <c r="AU28" s="25">
+      <c r="AU28" s="22">
         <v>232</v>
       </c>
-      <c r="AV28" s="26"/>
-      <c r="AW28" s="26"/>
-      <c r="AX28" s="26"/>
-      <c r="AY28" s="26"/>
-      <c r="AZ28" s="26"/>
-      <c r="BA28" s="26"/>
-      <c r="BB28" s="26"/>
-      <c r="BC28" s="27">
+      <c r="AV28" s="22">
+        <v>4643</v>
+      </c>
+      <c r="AW28" s="22">
+        <v>1018</v>
+      </c>
+      <c r="AX28" s="22">
+        <v>913</v>
+      </c>
+      <c r="AY28" s="22">
+        <v>1520</v>
+      </c>
+      <c r="AZ28" s="22">
+        <v>1013</v>
+      </c>
+      <c r="BA28" s="22">
+        <v>4736</v>
+      </c>
+      <c r="BB28" s="22">
+        <v>803</v>
+      </c>
+      <c r="BC28" s="19">
         <f t="shared" si="4"/>
-        <v>671</v>
+        <v>1665.9</v>
       </c>
     </row>
-    <row r="29" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29" s="16">
         <v>157</v>
       </c>
@@ -25346,7 +25640,7 @@
       <c r="AE29" s="21">
         <v>1009</v>
       </c>
-      <c r="AF29" s="23">
+      <c r="AF29" s="21">
         <v>152</v>
       </c>
       <c r="AG29" s="19">
@@ -25387,28 +25681,42 @@
         <f t="shared" si="0"/>
         <v>707.8</v>
       </c>
-      <c r="AS29" s="24">
+      <c r="AS29" s="22">
         <v>1779</v>
       </c>
-      <c r="AT29" s="24">
+      <c r="AT29" s="22">
         <v>231</v>
       </c>
-      <c r="AU29" s="25">
+      <c r="AU29" s="22">
         <v>800</v>
       </c>
-      <c r="AV29" s="26"/>
-      <c r="AW29" s="26"/>
-      <c r="AX29" s="26"/>
-      <c r="AY29" s="26"/>
-      <c r="AZ29" s="26"/>
-      <c r="BA29" s="26"/>
-      <c r="BB29" s="26"/>
-      <c r="BC29" s="27">
+      <c r="AV29" s="22">
+        <v>4626</v>
+      </c>
+      <c r="AW29" s="22">
+        <v>4517</v>
+      </c>
+      <c r="AX29" s="22">
+        <v>1013</v>
+      </c>
+      <c r="AY29" s="22">
+        <v>232</v>
+      </c>
+      <c r="AZ29" s="22">
+        <v>750</v>
+      </c>
+      <c r="BA29" s="22">
+        <v>4766</v>
+      </c>
+      <c r="BB29" s="22">
+        <v>911</v>
+      </c>
+      <c r="BC29" s="19">
         <f t="shared" si="4"/>
-        <v>936.66666666666663</v>
+        <v>1962.5</v>
       </c>
     </row>
-    <row r="30" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A30" s="16">
         <v>154</v>
       </c>
@@ -25504,7 +25812,7 @@
       <c r="AE30" s="21">
         <v>1068</v>
       </c>
-      <c r="AF30" s="23">
+      <c r="AF30" s="21">
         <v>231</v>
       </c>
       <c r="AG30" s="19">
@@ -25545,28 +25853,42 @@
         <f t="shared" si="0"/>
         <v>713.6</v>
       </c>
-      <c r="AS30" s="24">
+      <c r="AS30" s="22">
         <v>1762</v>
       </c>
-      <c r="AT30" s="24">
+      <c r="AT30" s="22">
         <v>232</v>
       </c>
-      <c r="AU30" s="25">
+      <c r="AU30" s="22">
         <v>910</v>
       </c>
-      <c r="AV30" s="26"/>
-      <c r="AW30" s="26"/>
-      <c r="AX30" s="26"/>
-      <c r="AY30" s="26"/>
-      <c r="AZ30" s="26"/>
-      <c r="BA30" s="26"/>
-      <c r="BB30" s="26"/>
-      <c r="BC30" s="27">
+      <c r="AV30" s="22">
+        <v>4682</v>
+      </c>
+      <c r="AW30" s="22">
+        <v>4476</v>
+      </c>
+      <c r="AX30" s="22">
+        <v>961</v>
+      </c>
+      <c r="AY30" s="22">
+        <v>1010</v>
+      </c>
+      <c r="AZ30" s="22">
+        <v>1011</v>
+      </c>
+      <c r="BA30" s="22">
+        <v>4752</v>
+      </c>
+      <c r="BB30" s="22">
+        <v>1066</v>
+      </c>
+      <c r="BC30" s="19">
         <f t="shared" si="4"/>
-        <v>968</v>
+        <v>2086.1999999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31" s="16">
         <v>156</v>
       </c>
@@ -25662,7 +25984,7 @@
       <c r="AE31" s="21">
         <v>910</v>
       </c>
-      <c r="AF31" s="23">
+      <c r="AF31" s="21">
         <v>230</v>
       </c>
       <c r="AG31" s="19">
@@ -25703,28 +26025,42 @@
         <f t="shared" si="0"/>
         <v>766.9</v>
       </c>
-      <c r="AS31" s="24">
+      <c r="AS31" s="22">
         <v>1944</v>
       </c>
-      <c r="AT31" s="24">
+      <c r="AT31" s="22">
         <v>151</v>
       </c>
-      <c r="AU31" s="25">
+      <c r="AU31" s="22">
         <v>807</v>
       </c>
-      <c r="AV31" s="26"/>
-      <c r="AW31" s="26"/>
-      <c r="AX31" s="26"/>
-      <c r="AY31" s="26"/>
-      <c r="AZ31" s="26"/>
-      <c r="BA31" s="26"/>
-      <c r="BB31" s="26"/>
-      <c r="BC31" s="27">
+      <c r="AV31" s="22">
+        <v>4631</v>
+      </c>
+      <c r="AW31" s="22">
+        <v>4539</v>
+      </c>
+      <c r="AX31" s="22">
+        <v>1021</v>
+      </c>
+      <c r="AY31" s="22">
+        <v>441</v>
+      </c>
+      <c r="AZ31" s="22">
+        <v>1545</v>
+      </c>
+      <c r="BA31" s="22">
+        <v>4710</v>
+      </c>
+      <c r="BB31" s="22">
+        <v>858</v>
+      </c>
+      <c r="BC31" s="19">
         <f t="shared" si="4"/>
-        <v>967.33333333333337</v>
+        <v>2064.6999999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" s="16">
         <v>154</v>
       </c>
@@ -25820,7 +26156,7 @@
       <c r="AE32" s="21">
         <v>917</v>
       </c>
-      <c r="AF32" s="23">
+      <c r="AF32" s="21">
         <v>150</v>
       </c>
       <c r="AG32" s="19">
@@ -25861,28 +26197,42 @@
         <f t="shared" si="0"/>
         <v>850.9</v>
       </c>
-      <c r="AS32" s="24">
+      <c r="AS32" s="22">
         <v>1834</v>
       </c>
-      <c r="AT32" s="24">
+      <c r="AT32" s="22">
         <v>150</v>
       </c>
-      <c r="AU32" s="25">
+      <c r="AU32" s="22">
         <v>809</v>
       </c>
-      <c r="AV32" s="26"/>
-      <c r="AW32" s="26"/>
-      <c r="AX32" s="26"/>
-      <c r="AY32" s="26"/>
-      <c r="AZ32" s="26"/>
-      <c r="BA32" s="26"/>
-      <c r="BB32" s="26"/>
-      <c r="BC32" s="27">
+      <c r="AV32" s="22">
+        <v>4650</v>
+      </c>
+      <c r="AW32" s="22">
+        <v>4627</v>
+      </c>
+      <c r="AX32" s="22">
+        <v>967</v>
+      </c>
+      <c r="AY32" s="22">
+        <v>633</v>
+      </c>
+      <c r="AZ32" s="22">
+        <v>231</v>
+      </c>
+      <c r="BA32" s="22">
+        <v>4754</v>
+      </c>
+      <c r="BB32" s="22">
+        <v>910</v>
+      </c>
+      <c r="BC32" s="19">
         <f t="shared" si="4"/>
-        <v>931</v>
+        <v>1956.5</v>
       </c>
     </row>
-    <row r="33" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A33" s="16">
         <v>155</v>
       </c>
@@ -25978,7 +26328,7 @@
       <c r="AE33" s="21">
         <v>907</v>
       </c>
-      <c r="AF33" s="23">
+      <c r="AF33" s="21">
         <v>231</v>
       </c>
       <c r="AG33" s="19">
@@ -26019,28 +26369,42 @@
         <f t="shared" si="0"/>
         <v>775.8</v>
       </c>
-      <c r="AS33" s="24">
+      <c r="AS33" s="22">
         <v>4439</v>
       </c>
-      <c r="AT33" s="24">
+      <c r="AT33" s="22">
         <v>231</v>
       </c>
-      <c r="AU33" s="25">
+      <c r="AU33" s="22">
         <v>688</v>
       </c>
-      <c r="AV33" s="26"/>
-      <c r="AW33" s="26"/>
-      <c r="AX33" s="26"/>
-      <c r="AY33" s="26"/>
-      <c r="AZ33" s="26"/>
-      <c r="BA33" s="26"/>
-      <c r="BB33" s="26"/>
-      <c r="BC33" s="27">
+      <c r="AV33" s="22">
+        <v>4674</v>
+      </c>
+      <c r="AW33" s="22">
+        <v>4591</v>
+      </c>
+      <c r="AX33" s="22">
+        <v>1020</v>
+      </c>
+      <c r="AY33" s="22">
+        <v>912</v>
+      </c>
+      <c r="AZ33" s="22">
+        <v>442</v>
+      </c>
+      <c r="BA33" s="22">
+        <v>4810</v>
+      </c>
+      <c r="BB33" s="22">
+        <v>964</v>
+      </c>
+      <c r="BC33" s="19">
         <f t="shared" si="4"/>
-        <v>1786</v>
+        <v>2277.1</v>
       </c>
     </row>
-    <row r="34" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A34" s="16">
         <v>153</v>
       </c>
@@ -26136,7 +26500,7 @@
       <c r="AE34" s="21">
         <v>914</v>
       </c>
-      <c r="AF34" s="23">
+      <c r="AF34" s="21">
         <v>232</v>
       </c>
       <c r="AG34" s="19">
@@ -26177,28 +26541,42 @@
         <f t="shared" si="0"/>
         <v>702</v>
       </c>
-      <c r="AS34" s="24">
+      <c r="AS34" s="22">
         <v>3987</v>
       </c>
-      <c r="AT34" s="24">
+      <c r="AT34" s="22">
         <v>233</v>
       </c>
-      <c r="AU34" s="25">
+      <c r="AU34" s="22">
         <v>1062</v>
       </c>
-      <c r="AV34" s="26"/>
-      <c r="AW34" s="26"/>
-      <c r="AX34" s="26"/>
-      <c r="AY34" s="26"/>
-      <c r="AZ34" s="26"/>
-      <c r="BA34" s="26"/>
-      <c r="BB34" s="26"/>
-      <c r="BC34" s="27">
+      <c r="AV34" s="22">
+        <v>4610</v>
+      </c>
+      <c r="AW34" s="22">
+        <v>4443</v>
+      </c>
+      <c r="AX34" s="22">
+        <v>1012</v>
+      </c>
+      <c r="AY34" s="22">
+        <v>1017</v>
+      </c>
+      <c r="AZ34" s="22">
+        <v>306</v>
+      </c>
+      <c r="BA34" s="22">
+        <v>4667</v>
+      </c>
+      <c r="BB34" s="22">
+        <v>910</v>
+      </c>
+      <c r="BC34" s="19">
         <f t="shared" si="4"/>
-        <v>1760.6666666666667</v>
+        <v>2224.6999999999998</v>
       </c>
     </row>
-    <row r="35" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A35" s="16">
         <v>155</v>
       </c>
@@ -26294,7 +26672,7 @@
       <c r="AE35" s="21">
         <v>695</v>
       </c>
-      <c r="AF35" s="23">
+      <c r="AF35" s="21">
         <v>234</v>
       </c>
       <c r="AG35" s="19">
@@ -26335,28 +26713,42 @@
         <f t="shared" si="0"/>
         <v>860.3</v>
       </c>
-      <c r="AS35" s="24">
+      <c r="AS35" s="22">
         <v>3412</v>
       </c>
-      <c r="AT35" s="24">
+      <c r="AT35" s="22">
         <v>233</v>
       </c>
-      <c r="AU35" s="25">
+      <c r="AU35" s="22">
         <v>298</v>
       </c>
-      <c r="AV35" s="26"/>
-      <c r="AW35" s="26"/>
-      <c r="AX35" s="26"/>
-      <c r="AY35" s="26"/>
-      <c r="AZ35" s="26"/>
-      <c r="BA35" s="26"/>
-      <c r="BB35" s="26"/>
-      <c r="BC35" s="27">
+      <c r="AV35" s="22">
+        <v>4584</v>
+      </c>
+      <c r="AW35" s="22">
+        <v>4595</v>
+      </c>
+      <c r="AX35" s="22">
+        <v>911</v>
+      </c>
+      <c r="AY35" s="22">
+        <v>912</v>
+      </c>
+      <c r="AZ35" s="22">
+        <v>225</v>
+      </c>
+      <c r="BA35" s="22">
+        <v>4727</v>
+      </c>
+      <c r="BB35" s="22">
+        <v>909</v>
+      </c>
+      <c r="BC35" s="19">
         <f t="shared" si="4"/>
-        <v>1314.3333333333333</v>
+        <v>2080.6</v>
       </c>
     </row>
-    <row r="36" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A36" s="16">
         <v>154</v>
       </c>
@@ -26452,7 +26844,7 @@
       <c r="AE36" s="21">
         <v>753</v>
       </c>
-      <c r="AF36" s="23">
+      <c r="AF36" s="21">
         <v>231</v>
       </c>
       <c r="AG36" s="19">
@@ -26493,28 +26885,42 @@
         <f t="shared" si="0"/>
         <v>799.7</v>
       </c>
-      <c r="AS36" s="24">
+      <c r="AS36" s="22">
         <v>4585</v>
       </c>
-      <c r="AT36" s="24">
+      <c r="AT36" s="22">
         <v>440</v>
       </c>
-      <c r="AU36" s="25">
+      <c r="AU36" s="22">
         <v>1514</v>
       </c>
-      <c r="AV36" s="26"/>
-      <c r="AW36" s="26"/>
-      <c r="AX36" s="26"/>
-      <c r="AY36" s="26"/>
-      <c r="AZ36" s="26"/>
-      <c r="BA36" s="26"/>
-      <c r="BB36" s="26"/>
-      <c r="BC36" s="27">
+      <c r="AV36" s="22">
+        <v>4648</v>
+      </c>
+      <c r="AW36" s="22">
+        <v>4509</v>
+      </c>
+      <c r="AX36" s="22">
+        <v>1065</v>
+      </c>
+      <c r="AY36" s="22">
+        <v>965</v>
+      </c>
+      <c r="AZ36" s="22">
+        <v>507</v>
+      </c>
+      <c r="BA36" s="22">
+        <v>4776</v>
+      </c>
+      <c r="BB36" s="22">
+        <v>911</v>
+      </c>
+      <c r="BC36" s="19">
         <f t="shared" si="4"/>
-        <v>2179.6666666666665</v>
+        <v>2392</v>
       </c>
     </row>
-    <row r="37" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A37" s="16">
         <v>153</v>
       </c>
@@ -26610,7 +27016,7 @@
       <c r="AE37" s="21">
         <v>911</v>
       </c>
-      <c r="AF37" s="23">
+      <c r="AF37" s="21">
         <v>235</v>
       </c>
       <c r="AG37" s="19">
@@ -26651,28 +27057,42 @@
         <f t="shared" si="0"/>
         <v>878.5</v>
       </c>
-      <c r="AS37" s="24">
+      <c r="AS37" s="22">
         <v>1942</v>
       </c>
-      <c r="AT37" s="24">
+      <c r="AT37" s="22">
         <v>507</v>
       </c>
-      <c r="AU37" s="25">
+      <c r="AU37" s="22">
         <v>811</v>
       </c>
-      <c r="AV37" s="26"/>
-      <c r="AW37" s="26"/>
-      <c r="AX37" s="26"/>
-      <c r="AY37" s="26"/>
-      <c r="AZ37" s="26"/>
-      <c r="BA37" s="26"/>
-      <c r="BB37" s="26"/>
-      <c r="BC37" s="27">
+      <c r="AV37" s="22">
+        <v>4620</v>
+      </c>
+      <c r="AW37" s="22">
+        <v>4644</v>
+      </c>
+      <c r="AX37" s="22">
+        <v>907</v>
+      </c>
+      <c r="AY37" s="22">
+        <v>909</v>
+      </c>
+      <c r="AZ37" s="22">
+        <v>1011</v>
+      </c>
+      <c r="BA37" s="22">
+        <v>4780</v>
+      </c>
+      <c r="BB37" s="22">
+        <v>749</v>
+      </c>
+      <c r="BC37" s="19">
         <f t="shared" si="4"/>
-        <v>1086.6666666666667</v>
+        <v>2088</v>
       </c>
     </row>
-    <row r="38" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A38" s="16">
         <v>161</v>
       </c>
@@ -26768,7 +27188,7 @@
       <c r="AE38" s="21">
         <v>568</v>
       </c>
-      <c r="AF38" s="23">
+      <c r="AF38" s="21">
         <v>151</v>
       </c>
       <c r="AG38" s="19">
@@ -26806,31 +27226,45 @@
         <v>913</v>
       </c>
       <c r="AR38" s="19">
-        <f t="shared" ref="AR38:AR69" si="5">AVERAGE(AH38:AQ38)</f>
+        <f t="shared" ref="AR38:AR55" si="5">AVERAGE(AH38:AQ38)</f>
         <v>656.4</v>
       </c>
-      <c r="AS38" s="24">
+      <c r="AS38" s="22">
         <v>1979</v>
       </c>
-      <c r="AT38" s="24">
+      <c r="AT38" s="22">
         <v>566</v>
       </c>
-      <c r="AU38" s="25">
+      <c r="AU38" s="22">
         <v>911</v>
       </c>
-      <c r="AV38" s="26"/>
-      <c r="AW38" s="26"/>
-      <c r="AX38" s="26"/>
-      <c r="AY38" s="26"/>
-      <c r="AZ38" s="26"/>
-      <c r="BA38" s="26"/>
-      <c r="BB38" s="26"/>
-      <c r="BC38" s="27">
+      <c r="AV38" s="22">
+        <v>4609</v>
+      </c>
+      <c r="AW38" s="22">
+        <v>4464</v>
+      </c>
+      <c r="AX38" s="22">
+        <v>691</v>
+      </c>
+      <c r="AY38" s="22">
+        <v>1566</v>
+      </c>
+      <c r="AZ38" s="22">
+        <v>1016</v>
+      </c>
+      <c r="BA38" s="22">
+        <v>4726</v>
+      </c>
+      <c r="BB38" s="22">
+        <v>1160</v>
+      </c>
+      <c r="BC38" s="19">
         <f t="shared" si="4"/>
-        <v>1152</v>
+        <v>2168.8000000000002</v>
       </c>
     </row>
-    <row r="39" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A39" s="16">
         <v>156</v>
       </c>
@@ -26926,7 +27360,7 @@
       <c r="AE39" s="21">
         <v>1211</v>
       </c>
-      <c r="AF39" s="23">
+      <c r="AF39" s="21">
         <v>234</v>
       </c>
       <c r="AG39" s="19">
@@ -26967,28 +27401,42 @@
         <f t="shared" si="5"/>
         <v>721.6</v>
       </c>
-      <c r="AS39" s="24">
+      <c r="AS39" s="22">
         <v>498</v>
       </c>
-      <c r="AT39" s="24">
+      <c r="AT39" s="22">
         <v>908</v>
       </c>
-      <c r="AU39" s="25">
+      <c r="AU39" s="22">
         <v>968</v>
       </c>
-      <c r="AV39" s="26"/>
-      <c r="AW39" s="26"/>
-      <c r="AX39" s="26"/>
-      <c r="AY39" s="26"/>
-      <c r="AZ39" s="26"/>
-      <c r="BA39" s="26"/>
-      <c r="BB39" s="26"/>
-      <c r="BC39" s="27">
+      <c r="AV39" s="22">
+        <v>4646</v>
+      </c>
+      <c r="AW39" s="22">
+        <v>4449</v>
+      </c>
+      <c r="AX39" s="22">
+        <v>622</v>
+      </c>
+      <c r="AY39" s="22">
+        <v>860</v>
+      </c>
+      <c r="AZ39" s="22">
+        <v>693</v>
+      </c>
+      <c r="BA39" s="22">
+        <v>4774</v>
+      </c>
+      <c r="BB39" s="22">
+        <v>964</v>
+      </c>
+      <c r="BC39" s="19">
         <f t="shared" si="4"/>
-        <v>791.33333333333337</v>
+        <v>1938.2</v>
       </c>
     </row>
-    <row r="40" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A40" s="16">
         <v>234</v>
       </c>
@@ -27084,7 +27532,7 @@
       <c r="AE40" s="21">
         <v>794</v>
       </c>
-      <c r="AF40" s="23">
+      <c r="AF40" s="21">
         <v>232</v>
       </c>
       <c r="AG40" s="19">
@@ -27125,28 +27573,42 @@
         <f t="shared" si="5"/>
         <v>781.8</v>
       </c>
-      <c r="AS40" s="24">
+      <c r="AS40" s="22">
         <v>689</v>
       </c>
-      <c r="AT40" s="24">
+      <c r="AT40" s="22">
         <v>566</v>
       </c>
-      <c r="AU40" s="25">
+      <c r="AU40" s="22">
         <v>1206</v>
       </c>
-      <c r="AV40" s="26"/>
-      <c r="AW40" s="26"/>
-      <c r="AX40" s="26"/>
-      <c r="AY40" s="26"/>
-      <c r="AZ40" s="26"/>
-      <c r="BA40" s="26"/>
-      <c r="BB40" s="26"/>
-      <c r="BC40" s="27">
+      <c r="AV40" s="22">
+        <v>4620</v>
+      </c>
+      <c r="AW40" s="22">
+        <v>4428</v>
+      </c>
+      <c r="AX40" s="22">
+        <v>957</v>
+      </c>
+      <c r="AY40" s="22">
+        <v>1160</v>
+      </c>
+      <c r="AZ40" s="22">
+        <v>910</v>
+      </c>
+      <c r="BA40" s="22">
+        <v>4683</v>
+      </c>
+      <c r="BB40" s="22">
+        <v>1062</v>
+      </c>
+      <c r="BC40" s="19">
         <f t="shared" si="4"/>
-        <v>820.33333333333337</v>
+        <v>2028.1</v>
       </c>
     </row>
-    <row r="41" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A41" s="16">
         <v>155</v>
       </c>
@@ -27242,7 +27704,7 @@
       <c r="AE41" s="21">
         <v>1298</v>
       </c>
-      <c r="AF41" s="23">
+      <c r="AF41" s="21">
         <v>232</v>
       </c>
       <c r="AG41" s="19">
@@ -27283,28 +27745,42 @@
         <f t="shared" si="5"/>
         <v>772.9</v>
       </c>
-      <c r="AS41" s="24">
+      <c r="AS41" s="22">
         <v>748</v>
       </c>
-      <c r="AT41" s="24">
+      <c r="AT41" s="22">
         <v>904</v>
       </c>
-      <c r="AU41" s="25">
+      <c r="AU41" s="22">
         <v>1111</v>
       </c>
-      <c r="AV41" s="26"/>
-      <c r="AW41" s="26"/>
-      <c r="AX41" s="26"/>
-      <c r="AY41" s="26"/>
-      <c r="AZ41" s="26"/>
-      <c r="BA41" s="26"/>
-      <c r="BB41" s="26"/>
-      <c r="BC41" s="27">
+      <c r="AV41" s="23">
+        <v>4620</v>
+      </c>
+      <c r="AW41" s="22">
+        <v>4432</v>
+      </c>
+      <c r="AX41" s="22">
+        <v>694</v>
+      </c>
+      <c r="AY41" s="22">
+        <v>960</v>
+      </c>
+      <c r="AZ41" s="22">
+        <v>695</v>
+      </c>
+      <c r="BA41" s="22">
+        <v>4704</v>
+      </c>
+      <c r="BB41" s="22">
+        <v>1211</v>
+      </c>
+      <c r="BC41" s="19">
         <f t="shared" si="4"/>
-        <v>921</v>
+        <v>2007.9</v>
       </c>
     </row>
-    <row r="42" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A42" s="16">
         <v>158</v>
       </c>
@@ -27400,7 +27876,7 @@
       <c r="AE42" s="21">
         <v>962</v>
       </c>
-      <c r="AF42" s="23">
+      <c r="AF42" s="21">
         <v>232</v>
       </c>
       <c r="AG42" s="19">
@@ -27441,28 +27917,42 @@
         <f t="shared" si="5"/>
         <v>890</v>
       </c>
-      <c r="AS42" s="24">
+      <c r="AS42" s="22">
         <v>686</v>
       </c>
-      <c r="AT42" s="24">
+      <c r="AT42" s="22">
         <v>568</v>
       </c>
-      <c r="AU42" s="25">
+      <c r="AU42" s="22">
         <v>1388</v>
       </c>
-      <c r="AV42" s="26"/>
-      <c r="AW42" s="26"/>
-      <c r="AX42" s="26"/>
-      <c r="AY42" s="26"/>
-      <c r="AZ42" s="26"/>
-      <c r="BA42" s="26"/>
-      <c r="BB42" s="26"/>
-      <c r="BC42" s="27">
+      <c r="AV42" s="23">
+        <v>4678</v>
+      </c>
+      <c r="AW42" s="22">
+        <v>4476</v>
+      </c>
+      <c r="AX42" s="22">
+        <v>911</v>
+      </c>
+      <c r="AY42" s="22">
+        <v>1016</v>
+      </c>
+      <c r="AZ42" s="22">
+        <v>1014</v>
+      </c>
+      <c r="BA42" s="22">
+        <v>4774</v>
+      </c>
+      <c r="BB42" s="22">
+        <v>962</v>
+      </c>
+      <c r="BC42" s="19">
         <f t="shared" si="4"/>
-        <v>880.66666666666663</v>
+        <v>2047.3</v>
       </c>
     </row>
-    <row r="43" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A43" s="16">
         <v>154</v>
       </c>
@@ -27558,7 +28048,7 @@
       <c r="AE43" s="21">
         <v>962</v>
       </c>
-      <c r="AF43" s="23">
+      <c r="AF43" s="21">
         <v>233</v>
       </c>
       <c r="AG43" s="19">
@@ -27599,28 +28089,42 @@
         <f t="shared" si="5"/>
         <v>775.3</v>
       </c>
-      <c r="AS43" s="24">
+      <c r="AS43" s="22">
         <v>507</v>
       </c>
-      <c r="AT43" s="24">
+      <c r="AT43" s="22">
         <v>1010</v>
       </c>
-      <c r="AU43" s="25">
+      <c r="AU43" s="22">
         <v>806</v>
       </c>
-      <c r="AV43" s="26"/>
-      <c r="AW43" s="26"/>
-      <c r="AX43" s="26"/>
-      <c r="AY43" s="26"/>
-      <c r="AZ43" s="26"/>
-      <c r="BA43" s="26"/>
-      <c r="BB43" s="26"/>
-      <c r="BC43" s="27">
+      <c r="AV43" s="23">
+        <v>4653</v>
+      </c>
+      <c r="AW43" s="22">
+        <v>4480</v>
+      </c>
+      <c r="AX43" s="22">
+        <v>689</v>
+      </c>
+      <c r="AY43" s="22">
+        <v>1424</v>
+      </c>
+      <c r="AZ43" s="22">
+        <v>857</v>
+      </c>
+      <c r="BA43" s="22">
+        <v>4740</v>
+      </c>
+      <c r="BB43" s="22">
+        <v>797</v>
+      </c>
+      <c r="BC43" s="19">
         <f t="shared" si="4"/>
-        <v>774.33333333333337</v>
+        <v>1996.3</v>
       </c>
     </row>
-    <row r="44" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A44" s="16">
         <v>225</v>
       </c>
@@ -27716,7 +28220,7 @@
       <c r="AE44" s="21">
         <v>1065</v>
       </c>
-      <c r="AF44" s="23">
+      <c r="AF44" s="21">
         <v>231</v>
       </c>
       <c r="AG44" s="19">
@@ -27757,28 +28261,42 @@
         <f t="shared" si="5"/>
         <v>751.8</v>
       </c>
-      <c r="AS44" s="24">
+      <c r="AS44" s="22">
         <v>690</v>
       </c>
-      <c r="AT44" s="24">
+      <c r="AT44" s="22">
         <v>1012</v>
       </c>
-      <c r="AU44" s="25">
+      <c r="AU44" s="22">
         <v>960</v>
       </c>
-      <c r="AV44" s="26"/>
-      <c r="AW44" s="26"/>
-      <c r="AX44" s="26"/>
-      <c r="AY44" s="26"/>
-      <c r="AZ44" s="26"/>
-      <c r="BA44" s="26"/>
-      <c r="BB44" s="26"/>
-      <c r="BC44" s="27">
+      <c r="AV44" s="23">
+        <v>4621</v>
+      </c>
+      <c r="AW44" s="22">
+        <v>4652</v>
+      </c>
+      <c r="AX44" s="22">
+        <v>911</v>
+      </c>
+      <c r="AY44" s="22">
+        <v>910</v>
+      </c>
+      <c r="AZ44" s="22">
+        <v>798</v>
+      </c>
+      <c r="BA44" s="22">
+        <v>4742</v>
+      </c>
+      <c r="BB44" s="22">
+        <v>745</v>
+      </c>
+      <c r="BC44" s="19">
         <f t="shared" si="4"/>
-        <v>887.33333333333337</v>
+        <v>2004.1</v>
       </c>
     </row>
-    <row r="45" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A45" s="16">
         <v>153</v>
       </c>
@@ -27874,7 +28392,7 @@
       <c r="AE45" s="21">
         <v>1013</v>
       </c>
-      <c r="AF45" s="23">
+      <c r="AF45" s="21">
         <v>233</v>
       </c>
       <c r="AG45" s="19">
@@ -27915,28 +28433,42 @@
         <f t="shared" si="5"/>
         <v>731.8</v>
       </c>
-      <c r="AS45" s="24">
+      <c r="AS45" s="22">
         <v>571</v>
       </c>
-      <c r="AT45" s="24">
+      <c r="AT45" s="22">
         <v>1055</v>
       </c>
-      <c r="AU45" s="25">
+      <c r="AU45" s="22">
         <v>1019</v>
       </c>
-      <c r="AV45" s="26"/>
-      <c r="AW45" s="26"/>
-      <c r="AX45" s="26"/>
-      <c r="AY45" s="26"/>
-      <c r="AZ45" s="26"/>
-      <c r="BA45" s="26"/>
-      <c r="BB45" s="26"/>
-      <c r="BC45" s="27">
+      <c r="AV45" s="23">
+        <v>4611</v>
+      </c>
+      <c r="AW45" s="22">
+        <v>4564</v>
+      </c>
+      <c r="AX45" s="22">
+        <v>909</v>
+      </c>
+      <c r="AY45" s="22">
+        <v>1009</v>
+      </c>
+      <c r="AZ45" s="22">
+        <v>1254</v>
+      </c>
+      <c r="BA45" s="22">
+        <v>4746</v>
+      </c>
+      <c r="BB45" s="22">
+        <v>856</v>
+      </c>
+      <c r="BC45" s="19">
         <f t="shared" si="4"/>
-        <v>881.66666666666663</v>
+        <v>2059.4</v>
       </c>
     </row>
-    <row r="46" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A46" s="16">
         <v>158</v>
       </c>
@@ -28032,7 +28564,7 @@
       <c r="AE46" s="21">
         <v>1016</v>
       </c>
-      <c r="AF46" s="23">
+      <c r="AF46" s="21">
         <v>231</v>
       </c>
       <c r="AG46" s="19">
@@ -28073,28 +28605,42 @@
         <f t="shared" si="5"/>
         <v>810.2</v>
       </c>
-      <c r="AS46" s="24">
+      <c r="AS46" s="22">
         <v>625</v>
       </c>
-      <c r="AT46" s="24">
+      <c r="AT46" s="22">
         <v>1020</v>
       </c>
-      <c r="AU46" s="25">
+      <c r="AU46" s="22">
         <v>914</v>
       </c>
-      <c r="AV46" s="26"/>
-      <c r="AW46" s="26"/>
-      <c r="AX46" s="26"/>
-      <c r="AY46" s="26"/>
-      <c r="AZ46" s="26"/>
-      <c r="BA46" s="26"/>
-      <c r="BB46" s="26"/>
-      <c r="BC46" s="27">
+      <c r="AV46" s="23">
+        <v>4640</v>
+      </c>
+      <c r="AW46" s="22">
+        <v>4585</v>
+      </c>
+      <c r="AX46" s="22">
+        <v>967</v>
+      </c>
+      <c r="AY46" s="22">
+        <v>1117</v>
+      </c>
+      <c r="AZ46" s="22">
+        <v>1109</v>
+      </c>
+      <c r="BA46" s="22">
+        <v>4750</v>
+      </c>
+      <c r="BB46" s="22">
+        <v>690</v>
+      </c>
+      <c r="BC46" s="19">
         <f t="shared" si="4"/>
-        <v>853</v>
+        <v>2041.7</v>
       </c>
     </row>
-    <row r="47" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A47" s="16">
         <v>154</v>
       </c>
@@ -28190,7 +28736,7 @@
       <c r="AE47" s="21">
         <v>906</v>
       </c>
-      <c r="AF47" s="23">
+      <c r="AF47" s="21">
         <v>232</v>
       </c>
       <c r="AG47" s="19">
@@ -28231,28 +28777,42 @@
         <f t="shared" si="5"/>
         <v>679.5</v>
       </c>
-      <c r="AS47" s="24">
+      <c r="AS47" s="22">
         <v>626</v>
       </c>
-      <c r="AT47" s="24">
+      <c r="AT47" s="22">
         <v>1159</v>
       </c>
-      <c r="AU47" s="25">
+      <c r="AU47" s="22">
         <v>1012</v>
       </c>
-      <c r="AV47" s="26"/>
-      <c r="AW47" s="26"/>
-      <c r="AX47" s="26"/>
-      <c r="AY47" s="26"/>
-      <c r="AZ47" s="26"/>
-      <c r="BA47" s="26"/>
-      <c r="BB47" s="26"/>
-      <c r="BC47" s="27">
+      <c r="AV47" s="23">
+        <v>4610</v>
+      </c>
+      <c r="AW47" s="22">
+        <v>4580</v>
+      </c>
+      <c r="AX47" s="22">
+        <v>1067</v>
+      </c>
+      <c r="AY47" s="22">
+        <v>622</v>
+      </c>
+      <c r="AZ47" s="22">
+        <v>1069</v>
+      </c>
+      <c r="BA47" s="22">
+        <v>4781</v>
+      </c>
+      <c r="BB47" s="22">
+        <v>691</v>
+      </c>
+      <c r="BC47" s="19">
         <f t="shared" si="4"/>
-        <v>932.33333333333337</v>
+        <v>2021.7</v>
       </c>
     </row>
-    <row r="48" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A48" s="16">
         <v>161</v>
       </c>
@@ -28348,7 +28908,7 @@
       <c r="AE48" s="21">
         <v>1211</v>
       </c>
-      <c r="AF48" s="23">
+      <c r="AF48" s="21">
         <v>231</v>
       </c>
       <c r="AG48" s="19">
@@ -28389,28 +28949,42 @@
         <f t="shared" si="5"/>
         <v>770.5</v>
       </c>
-      <c r="AS48" s="24">
+      <c r="AS48" s="22">
         <v>1015</v>
       </c>
-      <c r="AT48" s="24">
+      <c r="AT48" s="22">
         <v>1013</v>
       </c>
-      <c r="AU48" s="25">
+      <c r="AU48" s="22">
         <v>916</v>
       </c>
-      <c r="AV48" s="26"/>
-      <c r="AW48" s="26"/>
-      <c r="AX48" s="26"/>
-      <c r="AY48" s="26"/>
-      <c r="AZ48" s="26"/>
-      <c r="BA48" s="26"/>
-      <c r="BB48" s="26"/>
-      <c r="BC48" s="27">
+      <c r="AV48" s="23">
+        <v>4612</v>
+      </c>
+      <c r="AW48" s="22">
+        <v>4638</v>
+      </c>
+      <c r="AX48" s="22">
+        <v>1112</v>
+      </c>
+      <c r="AY48" s="22">
+        <v>858</v>
+      </c>
+      <c r="AZ48" s="22">
+        <v>1068</v>
+      </c>
+      <c r="BA48" s="22">
+        <v>4797</v>
+      </c>
+      <c r="BB48" s="22">
+        <v>686</v>
+      </c>
+      <c r="BC48" s="19">
         <f t="shared" si="4"/>
-        <v>981.33333333333337</v>
+        <v>2071.5</v>
       </c>
     </row>
-    <row r="49" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A49" s="16">
         <v>225</v>
       </c>
@@ -28506,7 +29080,7 @@
       <c r="AE49" s="21">
         <v>807</v>
       </c>
-      <c r="AF49" s="23">
+      <c r="AF49" s="21">
         <v>231</v>
       </c>
       <c r="AG49" s="19">
@@ -28547,28 +29121,42 @@
         <f t="shared" si="5"/>
         <v>927.9</v>
       </c>
-      <c r="AS49" s="24">
+      <c r="AS49" s="22">
         <v>503</v>
       </c>
-      <c r="AT49" s="24">
+      <c r="AT49" s="22">
         <v>752</v>
       </c>
-      <c r="AU49" s="25">
+      <c r="AU49" s="22">
         <v>960</v>
       </c>
-      <c r="AV49" s="26"/>
-      <c r="AW49" s="26"/>
-      <c r="AX49" s="26"/>
-      <c r="AY49" s="26"/>
-      <c r="AZ49" s="26"/>
-      <c r="BA49" s="26"/>
-      <c r="BB49" s="26"/>
-      <c r="BC49" s="27">
+      <c r="AV49" s="23">
+        <v>4620</v>
+      </c>
+      <c r="AW49" s="22">
+        <v>4460</v>
+      </c>
+      <c r="AX49" s="22">
+        <v>1065</v>
+      </c>
+      <c r="AY49" s="22">
+        <v>854</v>
+      </c>
+      <c r="AZ49" s="22">
+        <v>1600</v>
+      </c>
+      <c r="BA49" s="22">
+        <v>4781</v>
+      </c>
+      <c r="BB49" s="22">
+        <v>629</v>
+      </c>
+      <c r="BC49" s="19">
         <f t="shared" si="4"/>
-        <v>738.33333333333337</v>
+        <v>2022.4</v>
       </c>
     </row>
-    <row r="50" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A50" s="16">
         <v>153</v>
       </c>
@@ -28664,7 +29252,7 @@
       <c r="AE50" s="21">
         <v>1014</v>
       </c>
-      <c r="AF50" s="23">
+      <c r="AF50" s="21">
         <v>150</v>
       </c>
       <c r="AG50" s="19">
@@ -28705,28 +29293,42 @@
         <f t="shared" si="5"/>
         <v>756.7</v>
       </c>
-      <c r="AS50" s="24">
+      <c r="AS50" s="22">
         <v>745</v>
       </c>
-      <c r="AT50" s="24">
+      <c r="AT50" s="22">
         <v>1005</v>
       </c>
-      <c r="AU50" s="25">
+      <c r="AU50" s="22">
         <v>1116</v>
       </c>
-      <c r="AV50" s="26"/>
-      <c r="AW50" s="26"/>
-      <c r="AX50" s="26"/>
-      <c r="AY50" s="26"/>
-      <c r="AZ50" s="26"/>
-      <c r="BA50" s="26"/>
-      <c r="BB50" s="26"/>
-      <c r="BC50" s="27">
+      <c r="AV50" s="23">
+        <v>4628</v>
+      </c>
+      <c r="AW50" s="22">
+        <v>4643</v>
+      </c>
+      <c r="AX50" s="22">
+        <v>958</v>
+      </c>
+      <c r="AY50" s="22">
+        <v>908</v>
+      </c>
+      <c r="AZ50" s="22">
+        <v>1057</v>
+      </c>
+      <c r="BA50" s="22">
+        <v>4744</v>
+      </c>
+      <c r="BB50" s="22">
+        <v>748</v>
+      </c>
+      <c r="BC50" s="19">
         <f t="shared" si="4"/>
-        <v>955.33333333333337</v>
+        <v>2055.1999999999998</v>
       </c>
     </row>
-    <row r="51" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A51" s="16">
         <v>153</v>
       </c>
@@ -28822,7 +29424,7 @@
       <c r="AE51" s="21">
         <v>1301</v>
       </c>
-      <c r="AF51" s="23">
+      <c r="AF51" s="21">
         <v>152</v>
       </c>
       <c r="AG51" s="19">
@@ -28863,28 +29465,42 @@
         <f t="shared" si="5"/>
         <v>778.4</v>
       </c>
-      <c r="AS51" s="24">
+      <c r="AS51" s="22">
         <v>692</v>
       </c>
-      <c r="AT51" s="24">
+      <c r="AT51" s="22">
         <v>690</v>
       </c>
-      <c r="AU51" s="25">
+      <c r="AU51" s="22">
         <v>915</v>
       </c>
-      <c r="AV51" s="26"/>
-      <c r="AW51" s="26"/>
-      <c r="AX51" s="26"/>
-      <c r="AY51" s="26"/>
-      <c r="AZ51" s="26"/>
-      <c r="BA51" s="26"/>
-      <c r="BB51" s="26"/>
-      <c r="BC51" s="27">
+      <c r="AV51" s="23">
+        <v>4646</v>
+      </c>
+      <c r="AW51" s="22">
+        <v>4605</v>
+      </c>
+      <c r="AX51" s="22">
+        <v>1012</v>
+      </c>
+      <c r="AY51" s="22">
+        <v>625</v>
+      </c>
+      <c r="AZ51" s="22">
+        <v>1196</v>
+      </c>
+      <c r="BA51" s="22">
+        <v>4751</v>
+      </c>
+      <c r="BB51" s="22">
+        <v>694</v>
+      </c>
+      <c r="BC51" s="19">
         <f t="shared" si="4"/>
-        <v>765.66666666666663</v>
+        <v>1982.6</v>
       </c>
     </row>
-    <row r="52" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A52" s="16">
         <v>155</v>
       </c>
@@ -28980,7 +29596,7 @@
       <c r="AE52" s="21">
         <v>1505</v>
       </c>
-      <c r="AF52" s="23">
+      <c r="AF52" s="21">
         <v>232</v>
       </c>
       <c r="AG52" s="19">
@@ -29021,28 +29637,42 @@
         <f t="shared" si="5"/>
         <v>885.6</v>
       </c>
-      <c r="AS52" s="24">
+      <c r="AS52" s="22">
         <v>571</v>
       </c>
-      <c r="AT52" s="24">
+      <c r="AT52" s="22">
         <v>437</v>
       </c>
-      <c r="AU52" s="25">
+      <c r="AU52" s="22">
         <v>743</v>
       </c>
-      <c r="AV52" s="26"/>
-      <c r="AW52" s="26"/>
-      <c r="AX52" s="26"/>
-      <c r="AY52" s="26"/>
-      <c r="AZ52" s="26"/>
-      <c r="BA52" s="26"/>
-      <c r="BB52" s="26"/>
-      <c r="BC52" s="27">
+      <c r="AV52" s="23">
+        <v>4613</v>
+      </c>
+      <c r="AW52" s="22">
+        <v>4525</v>
+      </c>
+      <c r="AX52" s="22">
+        <v>737</v>
+      </c>
+      <c r="AY52" s="22">
+        <v>913</v>
+      </c>
+      <c r="AZ52" s="22">
+        <v>1206</v>
+      </c>
+      <c r="BA52" s="22">
+        <v>4729</v>
+      </c>
+      <c r="BB52" s="22">
+        <v>910</v>
+      </c>
+      <c r="BC52" s="19">
         <f t="shared" si="4"/>
-        <v>583.66666666666663</v>
+        <v>1938.4</v>
       </c>
     </row>
-    <row r="53" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A53" s="16">
         <v>153</v>
       </c>
@@ -29138,7 +29768,7 @@
       <c r="AE53" s="21">
         <v>1300</v>
       </c>
-      <c r="AF53" s="23">
+      <c r="AF53" s="21">
         <v>233</v>
       </c>
       <c r="AG53" s="19">
@@ -29179,28 +29809,42 @@
         <f t="shared" si="5"/>
         <v>865.7</v>
       </c>
-      <c r="AS53" s="24">
+      <c r="AS53" s="22">
         <v>696</v>
       </c>
-      <c r="AT53" s="24">
+      <c r="AT53" s="22">
         <v>630</v>
       </c>
-      <c r="AU53" s="25">
+      <c r="AU53" s="22">
         <v>749</v>
       </c>
-      <c r="AV53" s="26"/>
-      <c r="AW53" s="26"/>
-      <c r="AX53" s="26"/>
-      <c r="AY53" s="26"/>
-      <c r="AZ53" s="26"/>
-      <c r="BA53" s="26"/>
-      <c r="BB53" s="26"/>
-      <c r="BC53" s="27">
+      <c r="AV53" s="23">
+        <v>4623</v>
+      </c>
+      <c r="AW53" s="22">
+        <v>4626</v>
+      </c>
+      <c r="AX53" s="22">
+        <v>1519</v>
+      </c>
+      <c r="AY53" s="22">
+        <v>505</v>
+      </c>
+      <c r="AZ53" s="22">
+        <v>1205</v>
+      </c>
+      <c r="BA53" s="22">
+        <v>4742</v>
+      </c>
+      <c r="BB53" s="22">
+        <v>861</v>
+      </c>
+      <c r="BC53" s="19">
         <f t="shared" si="4"/>
-        <v>691.66666666666663</v>
+        <v>2015.6</v>
       </c>
     </row>
-    <row r="54" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A54" s="16">
         <v>156</v>
       </c>
@@ -29296,7 +29940,7 @@
       <c r="AE54" s="21">
         <v>628</v>
       </c>
-      <c r="AF54" s="23">
+      <c r="AF54" s="21">
         <v>232</v>
       </c>
       <c r="AG54" s="19">
@@ -29337,28 +29981,42 @@
         <f t="shared" si="5"/>
         <v>810.9</v>
       </c>
-      <c r="AS54" s="24">
+      <c r="AS54" s="22">
         <v>853</v>
       </c>
-      <c r="AT54" s="24">
+      <c r="AT54" s="22">
         <v>959</v>
       </c>
-      <c r="AU54" s="25">
+      <c r="AU54" s="22">
         <v>918</v>
       </c>
-      <c r="AV54" s="26"/>
-      <c r="AW54" s="26"/>
-      <c r="AX54" s="26"/>
-      <c r="AY54" s="26"/>
-      <c r="AZ54" s="26"/>
-      <c r="BA54" s="26"/>
-      <c r="BB54" s="26"/>
-      <c r="BC54" s="27">
+      <c r="AV54" s="23">
+        <v>4650</v>
+      </c>
+      <c r="AW54" s="22">
+        <v>4592</v>
+      </c>
+      <c r="AX54" s="22">
+        <v>963</v>
+      </c>
+      <c r="AY54" s="22">
+        <v>691</v>
+      </c>
+      <c r="AZ54" s="22">
+        <v>443</v>
+      </c>
+      <c r="BA54" s="22">
+        <v>4699</v>
+      </c>
+      <c r="BB54" s="22">
+        <v>1012</v>
+      </c>
+      <c r="BC54" s="19">
         <f t="shared" si="4"/>
-        <v>910</v>
+        <v>1978</v>
       </c>
     </row>
-    <row r="55" spans="1:55" ht="16" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A55" s="16">
         <v>155</v>
       </c>
@@ -29454,7 +30112,7 @@
       <c r="AE55" s="21">
         <v>861</v>
       </c>
-      <c r="AF55" s="23">
+      <c r="AF55" s="21">
         <v>232</v>
       </c>
       <c r="AG55" s="19">
@@ -29495,28 +30153,42 @@
         <f t="shared" si="5"/>
         <v>882.1</v>
       </c>
-      <c r="AS55" s="24">
+      <c r="AS55" s="22">
         <v>744</v>
       </c>
-      <c r="AT55" s="24">
+      <c r="AT55" s="22">
         <v>1108</v>
       </c>
-      <c r="AU55" s="25">
+      <c r="AU55" s="22">
         <v>1021</v>
       </c>
-      <c r="AV55" s="26"/>
-      <c r="AW55" s="26"/>
-      <c r="AX55" s="26"/>
-      <c r="AY55" s="26"/>
-      <c r="AZ55" s="26"/>
-      <c r="BA55" s="26"/>
-      <c r="BB55" s="26"/>
-      <c r="BC55" s="27">
+      <c r="AV55" s="23">
+        <v>4621</v>
+      </c>
+      <c r="AW55" s="22">
+        <v>4545</v>
+      </c>
+      <c r="AX55" s="22">
+        <v>1255</v>
+      </c>
+      <c r="AY55" s="22">
+        <v>634</v>
+      </c>
+      <c r="AZ55" s="22">
+        <v>801</v>
+      </c>
+      <c r="BA55" s="22">
+        <v>4728</v>
+      </c>
+      <c r="BB55" s="22">
+        <v>914</v>
+      </c>
+      <c r="BC55" s="19">
         <f t="shared" si="4"/>
-        <v>957.66666666666663</v>
+        <v>2037.1</v>
       </c>
     </row>
-    <row r="56" spans="1:55" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:55" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
         <v>46</v>
       </c>
@@ -29563,17 +30235,17 @@
       <c r="AP56" s="5"/>
       <c r="AQ56" s="5"/>
       <c r="AR56" s="5"/>
-      <c r="AS56" s="22"/>
-      <c r="AT56" s="22"/>
-      <c r="AU56" s="22"/>
-      <c r="AV56" s="22"/>
-      <c r="AW56" s="22"/>
-      <c r="AX56" s="22"/>
-      <c r="AY56" s="22"/>
-      <c r="AZ56" s="22"/>
-      <c r="BA56" s="22"/>
-      <c r="BB56" s="22"/>
-      <c r="BC56" s="22"/>
+      <c r="AS56" s="5"/>
+      <c r="AT56" s="5"/>
+      <c r="AU56" s="5"/>
+      <c r="AV56" s="5"/>
+      <c r="AW56" s="5"/>
+      <c r="AX56" s="5"/>
+      <c r="AY56" s="5"/>
+      <c r="AZ56" s="5"/>
+      <c r="BA56" s="5"/>
+      <c r="BB56" s="5"/>
+      <c r="BC56" s="5"/>
     </row>
     <row r="57" spans="1:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A57" s="2">
@@ -29763,41 +30435,41 @@
       </c>
       <c r="AV57" s="2">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>4682</v>
       </c>
       <c r="AW57" s="2">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>4652</v>
       </c>
       <c r="AX57" s="2">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1519</v>
       </c>
       <c r="AY57" s="2">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1566</v>
       </c>
       <c r="AZ57" s="2">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1761</v>
       </c>
       <c r="BA57" s="2">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>4828</v>
       </c>
       <c r="BB57" s="2">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1211</v>
       </c>
       <c r="BC57" s="2">
         <f t="shared" si="6"/>
-        <v>2179.6666666666665</v>
+        <v>2392</v>
       </c>
     </row>
     <row r="66" spans="29:31" x14ac:dyDescent="0.35">
       <c r="AD66">
         <f>_xlfn.T.TEST(AR6:AR55, BC6:BC55, 2,3)</f>
-        <v>2.187827294487099E-4</v>
+        <v>2.5635773599770767E-19</v>
       </c>
     </row>
     <row r="71" spans="29:31" x14ac:dyDescent="0.35">
@@ -29829,6 +30501,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>